<commit_message>
Excel graphs and layout left
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -2825,8 +2825,8 @@
   </sheetPr>
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D44" sqref="A1:D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -2899,10 +2899,10 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="110" t="n">
-        <v>42370</v>
+        <v>42736</v>
       </c>
       <c r="B2" s="110" t="n">
-        <v>42401</v>
+        <v>42767</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -2961,10 +2961,10 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="110" t="n">
-        <v>42401</v>
+        <v>42767</v>
       </c>
       <c r="B3" s="110" t="n">
-        <v>42430</v>
+        <v>42795</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -3023,10 +3023,10 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="110" t="n">
-        <v>42430</v>
+        <v>42795</v>
       </c>
       <c r="B4" s="110" t="n">
-        <v>42461</v>
+        <v>42826</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -3085,10 +3085,10 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="110" t="n">
-        <v>42461</v>
+        <v>42826</v>
       </c>
       <c r="B5" s="110" t="n">
-        <v>42490</v>
+        <v>42855</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
@@ -3147,10 +3147,10 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="110" t="n">
-        <v>42490</v>
+        <v>42855</v>
       </c>
       <c r="B6" s="110" t="n">
-        <v>42491</v>
+        <v>42856</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
@@ -3209,10 +3209,10 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="110" t="n">
-        <v>42491</v>
+        <v>42856</v>
       </c>
       <c r="B7" s="110" t="n">
-        <v>42522</v>
+        <v>42887</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
@@ -3271,10 +3271,10 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="110" t="n">
-        <v>42522</v>
+        <v>42887</v>
       </c>
       <c r="B8" s="110" t="n">
-        <v>42552</v>
+        <v>42917</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
@@ -3333,10 +3333,10 @@
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="110" t="n">
-        <v>42186</v>
+        <v>42552</v>
       </c>
       <c r="B9" s="110" t="n">
-        <v>42217</v>
+        <v>42583</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
@@ -3395,10 +3395,10 @@
     </row>
     <row r="10" spans="1:20">
       <c r="A10" s="110" t="n">
-        <v>42217</v>
+        <v>42583</v>
       </c>
       <c r="B10" s="110" t="n">
-        <v>42248</v>
+        <v>42614</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
@@ -3457,10 +3457,10 @@
     </row>
     <row r="11" spans="1:20">
       <c r="A11" s="110" t="n">
-        <v>42248</v>
+        <v>42614</v>
       </c>
       <c r="B11" s="110" t="n">
-        <v>42278</v>
+        <v>42644</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
@@ -3519,10 +3519,10 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="110" t="n">
-        <v>42278</v>
+        <v>42644</v>
       </c>
       <c r="B12" s="110" t="n">
-        <v>42309</v>
+        <v>42675</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
@@ -3581,10 +3581,10 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="110" t="n">
-        <v>42309</v>
+        <v>42675</v>
       </c>
       <c r="B13" s="110" t="n">
-        <v>42339</v>
+        <v>42705</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
@@ -3643,10 +3643,10 @@
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="110" t="n">
-        <v>42339</v>
+        <v>42705</v>
       </c>
       <c r="B14" s="110" t="n">
-        <v>42370</v>
+        <v>42736</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
@@ -3862,7 +3862,7 @@
         <v>47</v>
       </c>
       <c r="B34" t="n">
-        <v>22345.1531717015</v>
+        <v>22418.87716044388</v>
       </c>
       <c r="C34" t="s">
         <v>48</v>
@@ -3873,7 +3873,7 @@
         <v>49</v>
       </c>
       <c r="B35" t="n">
-        <v>0.1042836297487037</v>
+        <v>0.104627695644629</v>
       </c>
       <c r="C35" t="s">
         <v>50</v>
@@ -3895,7 +3895,7 @@
         <v>52</v>
       </c>
       <c r="B37" t="n">
-        <v>1.004093523131757</v>
+        <v>1.007406356972136</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
@@ -6801,8 +6801,8 @@
   </sheetPr>
   <dimension ref="A2:R307"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" view="pageBreakPreview" workbookViewId="0" zoomScale="25" zoomScaleNormal="25" zoomScalePageLayoutView="25" zoomScaleSheetLayoutView="25">
-      <selection activeCell="G141" sqref="G140:G141"/>
+    <sheetView view="pageBreakPreview" workbookViewId="0" zoomScale="25" zoomScaleNormal="25" zoomScalePageLayoutView="25" zoomScaleSheetLayoutView="25">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>

</xml_diff>